<commit_message>
fixed course upload and approval
</commit_message>
<xml_diff>
--- a/uploads/results/result_BCS28_BCME 206_semester_2_2024-2025.xlsx
+++ b/uploads/results/result_BCS28_BCME 206_semester_2_2024-2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\Desktop\2025 Exams Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rmu\staff\uploads\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551D9AC2-3A7F-4184-B569-39F4EC2C34C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CA1C5C-7080-49AA-9F2B-9441A60BCFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -992,7 +992,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>